<commit_message>
LMIC countries properly filtered, pop files now use bool instead of str
</commit_message>
<xml_diff>
--- a/misc/population.xlsx
+++ b/misc/population.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok Krishnamurthy\Desktop\ShinyDraft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB6FD2F-BADE-41F1-AFC3-E4C0A3795242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E78055-4200-4BBC-BDB0-D1A803AE7C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="171">
   <si>
     <t>Country</t>
   </si>
@@ -66,12 +66,6 @@
     <t>LMIC</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>Austria</t>
   </si>
   <si>
@@ -234,12 +228,6 @@
     <t>NLD</t>
   </si>
   <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>NOR</t>
-  </si>
-  <si>
     <t>Pakistan</t>
   </si>
   <si>
@@ -402,9 +390,6 @@
     <t>KEN</t>
   </si>
   <si>
-    <t>Lebanon</t>
-  </si>
-  <si>
     <t>LBN</t>
   </si>
   <si>
@@ -550,6 +535,15 @@
   </si>
   <si>
     <t>JPN</t>
+  </si>
+  <si>
+    <t>LebaFALSEn</t>
+  </si>
+  <si>
+    <t>FALSErway</t>
+  </si>
+  <si>
+    <t>FALSER</t>
   </si>
 </sst>
 </file>
@@ -842,18 +836,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C5C62-C8EE-4F49-9292-237310EC5B94}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -864,1180 +860,1180 @@
         <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>108</v>
+      </c>
+      <c r="C2" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D2" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>159</v>
+      </c>
+      <c r="C3" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D3" s="4">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D4" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D5" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D6" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D7" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D8" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D9" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="C10" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D10" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>12</v>
+        <v>110</v>
+      </c>
+      <c r="C11" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D11" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>11</v>
+        <v>161</v>
+      </c>
+      <c r="C12" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D12" s="4">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="C13" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D13" s="4">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
+      </c>
+      <c r="C14" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D14" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>11</v>
+        <v>30</v>
+      </c>
+      <c r="C15" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D15" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>11</v>
+      <c r="C16" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D16" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>12</v>
+      <c r="C17" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D17" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="C18" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D18" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>11</v>
+        <v>34</v>
+      </c>
+      <c r="C19" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D19" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>12</v>
+        <v>112</v>
+      </c>
+      <c r="C20" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D20" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>11</v>
+        <v>36</v>
+      </c>
+      <c r="C21" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D21" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>11</v>
+        <v>38</v>
+      </c>
+      <c r="C22" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D22" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>12</v>
+        <v>114</v>
+      </c>
+      <c r="C23" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D23" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>11</v>
+        <v>40</v>
+      </c>
+      <c r="C24" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D24" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>11</v>
+        <v>42</v>
+      </c>
+      <c r="C25" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D25" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>12</v>
+        <v>116</v>
+      </c>
+      <c r="C26" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D26" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>12</v>
+        <v>44</v>
+      </c>
+      <c r="C27" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D27" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>11</v>
+        <v>46</v>
+      </c>
+      <c r="C28" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D28" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>12</v>
+        <v>163</v>
+      </c>
+      <c r="C29" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D29" s="4">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>12</v>
+        <v>165</v>
+      </c>
+      <c r="C30" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D30" s="4">
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>11</v>
+        <v>48</v>
+      </c>
+      <c r="C31" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D31" s="4">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>11</v>
+        <v>50</v>
+      </c>
+      <c r="C32" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D32" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="C33" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D33" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>11</v>
+        <v>167</v>
+      </c>
+      <c r="C34" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D34" s="4">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>12</v>
+        <v>54</v>
+      </c>
+      <c r="C35" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D35" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>12</v>
+        <v>118</v>
+      </c>
+      <c r="C36" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D36" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>11</v>
+        <v>56</v>
+      </c>
+      <c r="C37" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D37" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>11</v>
+      <c r="C38" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D38" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>12</v>
+        <v>119</v>
+      </c>
+      <c r="C39" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D39" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>12</v>
+        <v>119</v>
+      </c>
+      <c r="C40" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D40" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>11</v>
+        <v>58</v>
+      </c>
+      <c r="C41" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D41" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>12</v>
+        <v>122</v>
+      </c>
+      <c r="C42" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D42" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>11</v>
+        <v>60</v>
+      </c>
+      <c r="C43" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D43" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>12</v>
+        <v>124</v>
+      </c>
+      <c r="C44" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D44" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>12</v>
+        <v>62</v>
+      </c>
+      <c r="C45" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D45" s="4">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>12</v>
+        <v>126</v>
+      </c>
+      <c r="C46" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D46" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>12</v>
+        <v>128</v>
+      </c>
+      <c r="C47" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D47" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>12</v>
+        <v>130</v>
+      </c>
+      <c r="C48" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D48" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>11</v>
+        <v>64</v>
+      </c>
+      <c r="C49" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D49" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>12</v>
+        <v>132</v>
+      </c>
+      <c r="C50" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D50" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>12</v>
+      <c r="C51" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D51" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>11</v>
+        <v>170</v>
+      </c>
+      <c r="C52" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D52" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>12</v>
+        <v>66</v>
+      </c>
+      <c r="C53" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D53" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>11</v>
+        <v>68</v>
+      </c>
+      <c r="C54" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D54" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>11</v>
+        <v>70</v>
+      </c>
+      <c r="C55" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D55" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>12</v>
+        <v>72</v>
+      </c>
+      <c r="C56" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D56" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>11</v>
+        <v>74</v>
+      </c>
+      <c r="C57" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D57" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>11</v>
+        <v>76</v>
+      </c>
+      <c r="C58" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D58" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>11</v>
+        <v>78</v>
+      </c>
+      <c r="C59" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D59" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>11</v>
+        <v>80</v>
+      </c>
+      <c r="C60" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D60" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>12</v>
+        <v>134</v>
+      </c>
+      <c r="C61" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D61" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>11</v>
+        <v>82</v>
+      </c>
+      <c r="C62" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D62" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>12</v>
+        <v>136</v>
+      </c>
+      <c r="C63" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D63" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>11</v>
+        <v>84</v>
+      </c>
+      <c r="C64" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D64" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>11</v>
+        <v>86</v>
+      </c>
+      <c r="C65" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D65" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>11</v>
+        <v>88</v>
+      </c>
+      <c r="C66" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D66" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>12</v>
+        <v>138</v>
+      </c>
+      <c r="C67" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D67" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>12</v>
+        <v>90</v>
+      </c>
+      <c r="C68" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D68" s="4">
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>11</v>
+        <v>92</v>
+      </c>
+      <c r="C69" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D69" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>12</v>
+        <v>140</v>
+      </c>
+      <c r="C70" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D70" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>11</v>
+        <v>94</v>
+      </c>
+      <c r="C71" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D71" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>12</v>
+        <v>96</v>
+      </c>
+      <c r="C72" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D72" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>12</v>
+        <v>142</v>
+      </c>
+      <c r="C73" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D73" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>12</v>
+        <v>144</v>
+      </c>
+      <c r="C74" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D74" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>11</v>
+        <v>98</v>
+      </c>
+      <c r="C75" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D75" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>11</v>
+        <v>100</v>
+      </c>
+      <c r="C76" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D76" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>12</v>
+        <v>146</v>
+      </c>
+      <c r="C77" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D77" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>12</v>
+        <v>148</v>
+      </c>
+      <c r="C78" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D78" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>12</v>
+        <v>150</v>
+      </c>
+      <c r="C79" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D79" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>11</v>
+        <v>102</v>
+      </c>
+      <c r="C80" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D80" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>12</v>
+        <v>152</v>
+      </c>
+      <c r="C81" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D81" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>12</v>
+        <v>104</v>
+      </c>
+      <c r="C82" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D82" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>11</v>
+        <v>106</v>
+      </c>
+      <c r="C83" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D83" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>12</v>
+        <v>154</v>
+      </c>
+      <c r="C84" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D84" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>12</v>
+        <v>156</v>
+      </c>
+      <c r="C85" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D85" s="4">
         <v>25</v>

</xml_diff>

<commit_message>
changed NGA aggregation factor 15 as default
</commit_message>
<xml_diff>
--- a/misc/population.xlsx
+++ b/misc/population.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok Krishnamurthy\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CD5766-237C-4924-8402-E080F62D65C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F781E0E6-E3E3-4BFB-8919-1EBAA5A37841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -573,12 +573,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -608,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -620,6 +626,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -843,9 +852,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -1061,16 +1070,16 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="C16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
         <v>10</v>
       </c>
     </row>
@@ -1551,17 +1560,17 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51" s="4">
-        <v>25</v>
+      <c r="C51" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" s="5">
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
minor R code changes
</commit_message>
<xml_diff>
--- a/misc/population.xlsx
+++ b/misc/population.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok Krishnamurthy\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F781E0E6-E3E3-4BFB-8919-1EBAA5A37841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6C837A-C312-4608-90FF-31053100EB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t>Country</t>
   </si>
@@ -511,12 +511,6 @@
   </si>
   <si>
     <t>ARG</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
-    <t>CHL</t>
   </si>
   <si>
     <t>India</t>
@@ -846,7 +840,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C5C62-C8EE-4F49-9292-237310EC5B94}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1015,38 +1009,38 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>160</v>
+        <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>161</v>
+        <v>26</v>
       </c>
       <c r="C12" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="4">
-        <v>95</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D13" s="4">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" s="4" t="b">
         <v>0</v>
@@ -1056,53 +1050,53 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="A15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5">
-        <v>10</v>
+      <c r="A16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4">
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C17" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="4">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C18" s="4" t="b">
         <v>0</v>
@@ -1113,80 +1107,80 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="C19" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>111</v>
+        <v>35</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
       <c r="C20" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C21" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D21" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="C22" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="4">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="C23" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C24" s="4" t="b">
         <v>0</v>
@@ -1197,58 +1191,58 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="C25" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="4">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>115</v>
+        <v>43</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>116</v>
+        <v>44</v>
       </c>
       <c r="C26" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D26" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C27" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>46</v>
+        <v>161</v>
       </c>
       <c r="C28" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="4">
-        <v>10</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1267,153 +1261,153 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>164</v>
+        <v>47</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>165</v>
+        <v>48</v>
       </c>
       <c r="C30" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" s="4">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C31" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D31" s="4">
-        <v>40</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C32" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D32" s="4">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>51</v>
+        <v>164</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>52</v>
+        <v>165</v>
       </c>
       <c r="C33" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D33" s="4">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>166</v>
+        <v>53</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>167</v>
+        <v>54</v>
       </c>
       <c r="C34" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="4">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="C35" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D35" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>118</v>
+        <v>56</v>
       </c>
       <c r="C36" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C37" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>3</v>
+        <v>166</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
       <c r="C38" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>119</v>
+        <v>169</v>
       </c>
       <c r="C39" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D39" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>171</v>
+        <v>58</v>
       </c>
       <c r="C40" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="4">
         <v>10</v>
@@ -1421,13 +1415,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>58</v>
+        <v>122</v>
       </c>
       <c r="C41" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" s="4">
         <v>10</v>
@@ -1435,587 +1429,587 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>121</v>
+        <v>59</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="C42" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" s="4">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="C43" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" s="4">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
       <c r="C44" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D44" s="4">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="C45" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D45" s="4">
-        <v>55</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C46" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D46" s="4">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C47" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D47" s="4">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>129</v>
+        <v>63</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>130</v>
+        <v>64</v>
       </c>
       <c r="C48" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>63</v>
+        <v>131</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>64</v>
+        <v>132</v>
       </c>
       <c r="C49" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" s="4">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C50" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50" s="4">
-        <v>35</v>
+      <c r="A50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" s="5">
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51" s="5">
-        <v>15</v>
+      <c r="A51" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51" s="4">
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>169</v>
+        <v>65</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>170</v>
+        <v>66</v>
       </c>
       <c r="C52" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" s="4">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C53" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" s="4">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C54" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D54" s="4">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C55" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55" s="4">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C56" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C57" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D57" s="4">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C58" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D58" s="4">
-        <v>45</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C59" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D59" s="4">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="C60" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>133</v>
+        <v>81</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="C61" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D61" s="4">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
       <c r="C62" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62" s="4">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>135</v>
+        <v>83</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
       <c r="C63" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C64" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D64" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C65" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D65" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="C66" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66" s="4">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
       <c r="C67" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D67" s="4">
-        <v>30</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C68" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" s="4">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="C69" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69" s="4">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="C70" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70" s="4">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C71" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D71" s="4">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>96</v>
+        <v>142</v>
       </c>
       <c r="C72" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D72" s="4">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C73" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D73" s="4">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="C74" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" s="4">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C75" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D75" s="4">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>99</v>
+        <v>145</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>100</v>
+        <v>146</v>
       </c>
       <c r="C76" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76" s="4">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C77" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D77" s="4">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C78" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D78" s="4">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="C79" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79" s="4">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>102</v>
+        <v>152</v>
       </c>
       <c r="C80" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80" s="4">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>152</v>
+        <v>104</v>
       </c>
       <c r="C81" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D81" s="4">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C82" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="C83" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D83" s="4">
         <v>25</v>
@@ -2023,10 +2017,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C84" s="4" t="b">
         <v>1</v>
@@ -2035,23 +2029,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C85" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D85" s="4">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C81">
-    <sortCondition ref="A2:A81"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C80">
+    <sortCondition ref="A2:A80"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
removed Argentina from list
</commit_message>
<xml_diff>
--- a/misc/population.xlsx
+++ b/misc/population.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok Krishnamurthy\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6C837A-C312-4608-90FF-31053100EB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1C031B-904F-482D-AFBA-048765FA993F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
   <si>
     <t>Country</t>
   </si>
@@ -505,18 +505,6 @@
   </si>
   <si>
     <t>reco_rasterAgg</t>
-  </si>
-  <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>ARG</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>IND</t>
   </si>
   <si>
     <t>Indonesia</t>
@@ -840,9 +828,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C5C62-C8EE-4F49-9292-237310EC5B94}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -883,27 +873,27 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>158</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>159</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="4">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="4">
         <v>10</v>
@@ -911,69 +901,69 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D6" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="4">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="4">
         <v>10</v>
@@ -981,52 +971,52 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
       <c r="C10" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D10" s="4">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="C11" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="4">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C12" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="4">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4" t="b">
         <v>0</v>
@@ -1036,53 +1026,53 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="A14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="5">
-        <v>10</v>
+      <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C16" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="4">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C17" s="4" t="b">
         <v>0</v>
@@ -1093,80 +1083,80 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="C18" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>111</v>
+        <v>35</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
       <c r="C19" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C20" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D20" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="C21" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="4">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="C22" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C23" s="4" t="b">
         <v>0</v>
@@ -1177,181 +1167,181 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="C24" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="4">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>115</v>
+        <v>43</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>116</v>
+        <v>44</v>
       </c>
       <c r="C25" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D25" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C26" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>46</v>
+        <v>159</v>
       </c>
       <c r="C27" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="4">
-        <v>10</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>160</v>
+        <v>47</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>161</v>
+        <v>48</v>
       </c>
       <c r="C28" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" s="4">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>162</v>
+        <v>49</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>163</v>
+        <v>50</v>
       </c>
       <c r="C29" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" s="4">
-        <v>65</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C30" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D30" s="4">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>49</v>
+        <v>160</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>50</v>
+        <v>161</v>
       </c>
       <c r="C31" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D31" s="4">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C32" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="4">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>164</v>
+        <v>117</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="C33" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="4">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C34" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>117</v>
+        <v>3</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>118</v>
+        <v>4</v>
       </c>
       <c r="C35" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" s="4">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>55</v>
+        <v>162</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="C36" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="4">
         <v>5</v>
@@ -1359,13 +1349,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>4</v>
+        <v>165</v>
       </c>
       <c r="C37" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="4">
         <v>10</v>
@@ -1373,24 +1363,24 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>166</v>
+        <v>57</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>119</v>
+        <v>58</v>
       </c>
       <c r="C38" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="C39" s="4" t="b">
         <v>1</v>
@@ -1401,181 +1391,181 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C40" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="4">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C41" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D41" s="4">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C42" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="4">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C43" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D43" s="4">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>62</v>
+        <v>128</v>
       </c>
       <c r="C44" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D44" s="4">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C45" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D45" s="4">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C46" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" s="4">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C47" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D47" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D48" s="5">
         <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D48" s="4">
-        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="C49" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" s="4">
         <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50" s="5">
-        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>168</v>
+        <v>68</v>
       </c>
       <c r="C51" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D51" s="4">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C52" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" s="4">
         <v>35</v>
@@ -1583,83 +1573,83 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C53" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C54" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D54" s="4">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C55" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55" s="4">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C56" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D56" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C57" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D57" s="4">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="C58" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58" s="4">
         <v>5</v>
@@ -1667,55 +1657,55 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C59" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D59" s="4">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C60" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D60" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C61" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D61" s="4">
-        <v>45</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="C62" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" s="4">
         <v>10</v>
@@ -1723,153 +1713,153 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C63" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D63" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="C64" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C65" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65" s="4">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>138</v>
+        <v>92</v>
       </c>
       <c r="C66" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" s="4">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="C67" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D67" s="4">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C68" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D68" s="4">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="C69" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D69" s="4">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="C70" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" s="4">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="C71" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D71" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="C72" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72" s="4">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>143</v>
+        <v>99</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="C73" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D73" s="4">
         <v>5</v>
@@ -1877,38 +1867,38 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="C74" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74" s="4">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="C75" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75" s="4">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C76" s="4" t="b">
         <v>1</v>
@@ -1919,13 +1909,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="C77" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D77" s="4">
         <v>25</v>
@@ -1933,10 +1923,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C78" s="4" t="b">
         <v>1</v>
@@ -1947,91 +1937,63 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C79" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="C80" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80" s="4">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>104</v>
+        <v>154</v>
       </c>
       <c r="C81" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D81" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>105</v>
+        <v>155</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>106</v>
+        <v>156</v>
       </c>
       <c r="C82" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C83" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D83" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C84" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D84" s="4">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C80">
-    <sortCondition ref="A2:A80"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C78">
+    <sortCondition ref="A2:A78"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
add new countries to dropdown list
</commit_message>
<xml_diff>
--- a/misc/population.xlsx
+++ b/misc/population.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok Krishnamurthy\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1C031B-904F-482D-AFBA-048765FA993F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700F803E-B87F-4135-9CC3-BAC9DB3ECEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="186">
   <si>
     <t>Country</t>
   </si>
@@ -529,6 +529,66 @@
   </si>
   <si>
     <t>LBR</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>DZA</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>BHR</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>EGY</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>ARE</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>GHA</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>HKG</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>JAM</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>PRY</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>ZWE</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -828,11 +888,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C5C62-C8EE-4F49-9292-237310EC5B94}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -859,41 +917,41 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>107</v>
+        <v>166</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="4" t="b">
-        <v>1</v>
+        <v>167</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="D2" s="4">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="C3" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4">
         <v>10</v>
@@ -901,349 +959,349 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>168</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="4" t="b">
-        <v>0</v>
+        <v>169</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="D5" s="4">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C7" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="4">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C8" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D8" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C9" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D9" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="4">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="4">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="C12" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="4">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D13" s="4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="5">
+      <c r="A14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="4">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="A16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="C17" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="4">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>111</v>
+        <v>31</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="C18" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="4">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>35</v>
+        <v>170</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="4" t="b">
-        <v>0</v>
+        <v>171</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="D19" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C20" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D20" s="4">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C21" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="4">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C22" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D22" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C23" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="4">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C24" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D24" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C25" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>45</v>
+        <v>174</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="4" t="b">
-        <v>0</v>
+        <v>175</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="D26" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>158</v>
+        <v>41</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>159</v>
+        <v>42</v>
       </c>
       <c r="C27" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="4">
-        <v>65</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>47</v>
+        <v>115</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="C28" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="4">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C29" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="4">
         <v>5</v>
@@ -1251,66 +1309,66 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>51</v>
+        <v>176</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="4" t="b">
-        <v>0</v>
+        <v>177</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="D30" s="4">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>160</v>
+        <v>45</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>161</v>
+        <v>46</v>
       </c>
       <c r="C31" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D31" s="4">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>53</v>
+        <v>158</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="C32" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D32" s="4">
-        <v>10</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="C33" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" s="4">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C34" s="4" t="b">
         <v>0</v>
@@ -1321,27 +1379,27 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="C35" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D35" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C36" s="4" t="b">
-        <v>1</v>
+        <v>179</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="D36" s="4">
         <v>5</v>
@@ -1349,27 +1407,27 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C37" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" s="4">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C38" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="4">
         <v>10</v>
@@ -1377,122 +1435,122 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C39" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D39" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C40" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="4">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="C41" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" s="4">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="C42" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D42" s="4">
-        <v>55</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>126</v>
+        <v>165</v>
       </c>
       <c r="C43" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D43" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>128</v>
+        <v>58</v>
       </c>
       <c r="C44" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" s="4">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C45" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D45" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C46" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D46" s="4">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C47" s="4" t="b">
         <v>1</v>
@@ -1502,109 +1560,109 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D48" s="5">
-        <v>15</v>
+      <c r="A48" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D48" s="4">
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="C49" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" s="4">
-        <v>45</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="C50" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D50" s="4">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>67</v>
+        <v>129</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>68</v>
+        <v>130</v>
       </c>
       <c r="C51" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C52" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D52" s="4">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>71</v>
+        <v>131</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="C53" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D53" s="4">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C54" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D54" s="4">
-        <v>20</v>
+      <c r="A54" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54" s="5">
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>75</v>
+        <v>163</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>76</v>
+        <v>164</v>
       </c>
       <c r="C55" s="4" t="b">
         <v>0</v>
@@ -1615,108 +1673,108 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C56" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56" s="4">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C57" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D57" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>133</v>
+        <v>180</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C58" s="4" t="b">
-        <v>1</v>
+        <v>181</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="D58" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C59" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D59" s="4">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
       <c r="C60" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D60" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C61" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D61" s="4">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C62" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D62" s="4">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C63" s="4" t="b">
         <v>0</v>
@@ -1727,83 +1785,83 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>137</v>
+        <v>79</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="C64" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D64" s="4">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
       <c r="C65" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D65" s="4">
-        <v>55</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C66" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D66" s="4">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C67" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D67" s="4">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C68" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D68" s="4">
-        <v>45</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C69" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69" s="4">
         <v>10</v>
@@ -1811,139 +1869,139 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>141</v>
+        <v>87</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>142</v>
+        <v>88</v>
       </c>
       <c r="C70" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70" s="4">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C71" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D71" s="4">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C72" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72" s="4">
-        <v>30</v>
+        <v>55</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C73" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D73" s="4">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C74" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D74" s="4">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>147</v>
+        <v>93</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
       <c r="C75" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D75" s="4">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>149</v>
+        <v>95</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>150</v>
+        <v>96</v>
       </c>
       <c r="C76" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D76" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="C77" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77" s="4">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C78" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D78" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C79" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79" s="4">
         <v>30</v>
@@ -1951,38 +2009,38 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C80" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D80" s="4">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C81" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D81" s="4">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C82" s="4" t="b">
         <v>1</v>
@@ -1991,9 +2049,135 @@
         <v>25</v>
       </c>
     </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C83" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D83" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C84" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D84" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C85" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D85" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C86" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D87" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C88" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D88" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C89" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D89" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C90" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D90" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D91" s="4">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C78">
-    <sortCondition ref="A2:A78"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D91">
+    <sortCondition ref="A2:A91"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
added new countries to dropdown list
</commit_message>
<xml_diff>
--- a/misc/population.xlsx
+++ b/misc/population.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok Krishnamurthy\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700F803E-B87F-4135-9CC3-BAC9DB3ECEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B04619-F2A8-45B0-AB54-C18840339AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>Country</t>
   </si>
@@ -583,12 +583,6 @@
   </si>
   <si>
     <t>ZWE</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -922,8 +916,8 @@
       <c r="B2" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>184</v>
+      <c r="C2" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D2" s="4">
         <v>45</v>
@@ -964,8 +958,8 @@
       <c r="B5" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>185</v>
+      <c r="C5" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1160,8 +1154,8 @@
       <c r="B19" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>184</v>
+      <c r="C19" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D19" s="4">
         <v>30</v>
@@ -1258,8 +1252,8 @@
       <c r="B26" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>184</v>
+      <c r="C26" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D26" s="4">
         <v>15</v>
@@ -1314,8 +1308,8 @@
       <c r="B30" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>185</v>
+      <c r="C30" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D30" s="4">
         <v>1</v>
@@ -1398,8 +1392,8 @@
       <c r="B36" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>184</v>
+      <c r="C36" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D36" s="4">
         <v>5</v>
@@ -1706,8 +1700,8 @@
       <c r="B58" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>184</v>
+      <c r="C58" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="D58" s="4">
         <v>20</v>
@@ -2112,8 +2106,8 @@
       <c r="B87" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>185</v>
+      <c r="C87" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D87" s="4">
         <v>10</v>
@@ -2168,8 +2162,8 @@
       <c r="B91" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C91" s="4" t="s">
-        <v>184</v>
+      <c r="C91" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="D91" s="4">
         <v>15</v>

</xml_diff>

<commit_message>
added 9 new countries and removed 2
</commit_message>
<xml_diff>
--- a/misc/population.xlsx
+++ b/misc/population.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok Krishnamurthy\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B04619-F2A8-45B0-AB54-C18840339AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE76D7B-7F7C-44C7-AAAB-747AE16A74A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
   <si>
     <t>Country</t>
   </si>
@@ -505,18 +505,6 @@
   </si>
   <si>
     <t>reco_rasterAgg</t>
-  </si>
-  <si>
-    <t>Indonesia</t>
-  </si>
-  <si>
-    <t>IDN</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>JPN</t>
   </si>
   <si>
     <t>Lebanon</t>
@@ -882,7 +870,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C5C62-C8EE-4F49-9292-237310EC5B94}">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -911,10 +899,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C2" s="4" t="b">
         <v>1</v>
@@ -953,10 +941,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
@@ -1149,10 +1137,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C19" s="4" t="b">
         <v>1</v>
@@ -1247,10 +1235,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C26" s="4" t="b">
         <v>1</v>
@@ -1303,10 +1291,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C30" s="4" t="b">
         <v>0</v>
@@ -1331,125 +1319,125 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>158</v>
+        <v>47</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>159</v>
+        <v>48</v>
       </c>
       <c r="C32" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="4">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C33" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D33" s="4">
-        <v>40</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C34" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D34" s="4">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>51</v>
+        <v>174</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>52</v>
+        <v>175</v>
       </c>
       <c r="C35" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="4">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>178</v>
+        <v>53</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>179</v>
+        <v>54</v>
       </c>
       <c r="C36" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D36" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>160</v>
+        <v>117</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>161</v>
+        <v>118</v>
       </c>
       <c r="C37" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="4">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C38" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>117</v>
+        <v>3</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>118</v>
+        <v>4</v>
       </c>
       <c r="C39" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" s="4">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>55</v>
+        <v>158</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="C40" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" s="4">
         <v>5</v>
@@ -1457,13 +1445,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>4</v>
+        <v>161</v>
       </c>
       <c r="C41" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" s="4">
         <v>10</v>
@@ -1471,24 +1459,24 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>162</v>
+        <v>57</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>119</v>
+        <v>58</v>
       </c>
       <c r="C42" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>165</v>
+        <v>122</v>
       </c>
       <c r="C43" s="4" t="b">
         <v>1</v>
@@ -1499,279 +1487,279 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C44" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D44" s="4">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C45" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D45" s="4">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C46" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" s="4">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C47" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D47" s="4">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>62</v>
+        <v>128</v>
       </c>
       <c r="C48" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D48" s="4">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C49" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D49" s="4">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C50" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" s="4">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C51" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D51" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52" s="5">
         <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C52" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D52" s="4">
-        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="C53" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54" s="4">
         <v>35</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D54" s="5">
-        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>163</v>
+        <v>67</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>164</v>
+        <v>68</v>
       </c>
       <c r="C55" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D55" s="4">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>65</v>
+        <v>176</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>66</v>
+        <v>177</v>
       </c>
       <c r="C56" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D56" s="4">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C57" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D57" s="4">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>180</v>
+        <v>71</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>181</v>
+        <v>72</v>
       </c>
       <c r="C58" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D58" s="4">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C59" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D59" s="4">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C60" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" s="4">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C61" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D61" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C62" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D62" s="4">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="C63" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63" s="4">
         <v>5</v>
@@ -1779,55 +1767,55 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C64" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D64" s="4">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C65" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D65" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C66" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D66" s="4">
-        <v>45</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="C67" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67" s="4">
         <v>10</v>
@@ -1835,153 +1823,153 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C68" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D68" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="C69" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69" s="4">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C70" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" s="4">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>138</v>
+        <v>92</v>
       </c>
       <c r="C71" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71" s="4">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="C72" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D72" s="4">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C73" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D73" s="4">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="C74" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D74" s="4">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="C75" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75" s="4">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="C76" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D76" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="C77" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D77" s="4">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>143</v>
+        <v>99</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="C78" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D78" s="4">
         <v>5</v>
@@ -1989,38 +1977,38 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="C79" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79" s="4">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="C80" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80" s="4">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C81" s="4" t="b">
         <v>1</v>
@@ -2031,13 +2019,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="C82" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82" s="4">
         <v>25</v>
@@ -2045,10 +2033,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C83" s="4" t="b">
         <v>1</v>
@@ -2059,69 +2047,69 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C84" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D84" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="C85" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D85" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C86" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" s="4">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="C87" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D87" s="4">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>105</v>
+        <v>155</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>106</v>
+        <v>156</v>
       </c>
       <c r="C88" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D88" s="4">
         <v>25</v>
@@ -2129,49 +2117,21 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="C89" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C90" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D90" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C91" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D91" s="4">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D91">
-    <sortCondition ref="A2:A91"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D89">
+    <sortCondition ref="A2:A89"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
modified list of countries
</commit_message>
<xml_diff>
--- a/misc/population.xlsx
+++ b/misc/population.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok Krishnamurthy\Desktop\spatialEpisim\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/948a51b5f5a6a0c9/Desktop/spatialEpisim/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE76D7B-7F7C-44C7-AAAB-747AE16A74A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{6FE76D7B-7F7C-44C7-AAAB-747AE16A74A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B320AED4-0025-4D41-8477-6846FA9368D8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
   <si>
     <t>Country</t>
   </si>
@@ -78,12 +78,6 @@
     <t>BGD</t>
   </si>
   <si>
-    <t>Belarus</t>
-  </si>
-  <si>
-    <t>BLR</t>
-  </si>
-  <si>
     <t>Belgium</t>
   </si>
   <si>
@@ -340,12 +334,6 @@
   </si>
   <si>
     <t>TUR</t>
-  </si>
-  <si>
-    <t>Ukraine</t>
-  </si>
-  <si>
-    <t>UKR</t>
   </si>
   <si>
     <t>United Kingdom</t>
@@ -870,20 +858,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C5C62-C8EE-4F49-9292-237310EC5B94}">
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="7.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -894,15 +882,15 @@
         <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C2" s="4" t="b">
         <v>1</v>
@@ -911,12 +899,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>1</v>
@@ -925,7 +913,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -939,12 +927,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
@@ -953,7 +941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -967,7 +955,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -978,10 +966,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -989,13 +977,13 @@
         <v>18</v>
       </c>
       <c r="C8" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1003,13 +991,13 @@
         <v>20</v>
       </c>
       <c r="C9" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -1017,41 +1005,41 @@
         <v>22</v>
       </c>
       <c r="C10" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>110</v>
-      </c>
       <c r="C12" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -1062,10 +1050,10 @@
         <v>0</v>
       </c>
       <c r="D13" s="4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -1079,105 +1067,105 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="C17" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>167</v>
-      </c>
       <c r="C19" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="C21" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
@@ -1188,122 +1176,122 @@
         <v>0</v>
       </c>
       <c r="D22" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D23" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="C24" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C26" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C28" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D28" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C29" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>173</v>
-      </c>
       <c r="C30" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D30" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>45</v>
       </c>
@@ -1314,10 +1302,10 @@
         <v>0</v>
       </c>
       <c r="D31" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>47</v>
       </c>
@@ -1328,10 +1316,10 @@
         <v>0</v>
       </c>
       <c r="D32" s="4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>49</v>
       </c>
@@ -1342,290 +1330,290 @@
         <v>0</v>
       </c>
       <c r="D33" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C34" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>175</v>
-      </c>
       <c r="C35" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D35" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D37" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="C42" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D43" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45" s="4">
         <v>55</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" s="4">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D39" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C40" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D40" s="4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D48" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D49" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C50" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C41" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D42" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C43" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D43" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D44" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C45" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D45" s="4">
+      <c r="B51" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D53" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D46" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C47" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D47" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C48" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D48" s="4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C49" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D49" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C50" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D50" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C51" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D52" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C53" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D53" s="4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>65</v>
       </c>
@@ -1633,41 +1621,41 @@
         <v>66</v>
       </c>
       <c r="C54" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C55" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D56" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C55" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D55" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C56" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D56" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>69</v>
       </c>
@@ -1675,13 +1663,13 @@
         <v>70</v>
       </c>
       <c r="C57" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>71</v>
       </c>
@@ -1689,13 +1677,13 @@
         <v>72</v>
       </c>
       <c r="C58" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>73</v>
       </c>
@@ -1706,10 +1694,10 @@
         <v>0</v>
       </c>
       <c r="D59" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>75</v>
       </c>
@@ -1720,10 +1708,10 @@
         <v>0</v>
       </c>
       <c r="D60" s="4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>77</v>
       </c>
@@ -1734,66 +1722,66 @@
         <v>0</v>
       </c>
       <c r="D61" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C62" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D62" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C62" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D62" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="C63" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C64" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D64" s="4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="C65" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>83</v>
       </c>
@@ -1804,10 +1792,10 @@
         <v>0</v>
       </c>
       <c r="D66" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>85</v>
       </c>
@@ -1818,38 +1806,38 @@
         <v>0</v>
       </c>
       <c r="D67" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D68" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C68" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D68" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="C69" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D69" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>89</v>
       </c>
@@ -1857,41 +1845,41 @@
         <v>90</v>
       </c>
       <c r="C70" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70" s="4">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D71" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C71" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D71" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>140</v>
-      </c>
       <c r="C72" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
         <v>93</v>
       </c>
@@ -1899,55 +1887,55 @@
         <v>94</v>
       </c>
       <c r="C73" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73" s="4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C74" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D74" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C75" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D75" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C74" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D74" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C75" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D75" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>144</v>
-      </c>
       <c r="C76" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D76" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
         <v>97</v>
       </c>
@@ -1958,180 +1946,152 @@
         <v>0</v>
       </c>
       <c r="D77" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C78" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D78" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C79" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D79" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C80" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D80" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C78" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D78" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C79" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D79" s="4">
+      <c r="C81" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D81" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C82" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D82" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C80" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D80" s="4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C83" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D83" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C84" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D84" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C81" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D81" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C82" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D82" s="4">
+      <c r="C85" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D85" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C83" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D83" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C84" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D84" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C85" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D85" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="C86" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="C87" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D87" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C88" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D88" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="C89" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D89" s="4">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D89">
-    <sortCondition ref="A2:A89"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D87">
+    <sortCondition ref="A2:A87"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
290623c Update: Decreases rec agg factor for DR Congo
</commit_message>
<xml_diff>
--- a/misc/population.xlsx
+++ b/misc/population.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/948a51b5f5a6a0c9/Desktop/spatialEpisim/misc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twhit957\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{6FE76D7B-7F7C-44C7-AAAB-747AE16A74A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B320AED4-0025-4D41-8477-6846FA9368D8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D05A2C4-EEB7-4584-9FE1-B575BEC2CCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -860,18 +860,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C5C62-C8EE-4F49-9292-237310EC5B94}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.90625" style="1"/>
+    <col min="3" max="3" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -885,7 +887,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>158</v>
       </c>
@@ -899,7 +901,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>103</v>
       </c>
@@ -913,7 +915,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -927,7 +929,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>160</v>
       </c>
@@ -941,7 +943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -955,7 +957,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -969,7 +971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -983,7 +985,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -997,7 +999,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -1011,7 +1013,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>105</v>
       </c>
@@ -1025,7 +1027,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -1039,7 +1041,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -1053,7 +1055,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -1067,7 +1069,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>1</v>
       </c>
@@ -1081,7 +1083,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1092,10 +1094,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
@@ -1109,7 +1111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>162</v>
       </c>
@@ -1123,7 +1125,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
@@ -1137,7 +1139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>107</v>
       </c>
@@ -1151,7 +1153,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1165,7 +1167,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
@@ -1179,7 +1181,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>109</v>
       </c>
@@ -1193,7 +1195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
@@ -1207,7 +1209,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>166</v>
       </c>
@@ -1221,7 +1223,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
@@ -1235,7 +1237,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>111</v>
       </c>
@@ -1249,7 +1251,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>41</v>
       </c>
@@ -1263,7 +1265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>168</v>
       </c>
@@ -1277,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>43</v>
       </c>
@@ -1291,7 +1293,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>45</v>
       </c>
@@ -1305,7 +1307,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>47</v>
       </c>
@@ -1319,7 +1321,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>49</v>
       </c>
@@ -1333,7 +1335,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>170</v>
       </c>
@@ -1347,7 +1349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>51</v>
       </c>
@@ -1361,7 +1363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>113</v>
       </c>
@@ -1375,7 +1377,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>53</v>
       </c>
@@ -1389,7 +1391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -1403,7 +1405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>154</v>
       </c>
@@ -1417,7 +1419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>116</v>
       </c>
@@ -1431,7 +1433,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>55</v>
       </c>
@@ -1445,7 +1447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>117</v>
       </c>
@@ -1459,7 +1461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>57</v>
       </c>
@@ -1473,7 +1475,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>119</v>
       </c>
@@ -1487,7 +1489,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>59</v>
       </c>
@@ -1501,7 +1503,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>121</v>
       </c>
@@ -1515,7 +1517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>123</v>
       </c>
@@ -1529,7 +1531,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>125</v>
       </c>
@@ -1543,7 +1545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>61</v>
       </c>
@@ -1557,7 +1559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>127</v>
       </c>
@@ -1571,7 +1573,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>5</v>
       </c>
@@ -1585,7 +1587,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>155</v>
       </c>
@@ -1599,7 +1601,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>63</v>
       </c>
@@ -1613,7 +1615,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>65</v>
       </c>
@@ -1627,7 +1629,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>172</v>
       </c>
@@ -1641,7 +1643,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>67</v>
       </c>
@@ -1655,7 +1657,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>69</v>
       </c>
@@ -1669,7 +1671,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>71</v>
       </c>
@@ -1683,7 +1685,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>73</v>
       </c>
@@ -1697,7 +1699,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>75</v>
       </c>
@@ -1711,7 +1713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>77</v>
       </c>
@@ -1725,7 +1727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>129</v>
       </c>
@@ -1739,7 +1741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>79</v>
       </c>
@@ -1753,7 +1755,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>131</v>
       </c>
@@ -1767,7 +1769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>81</v>
       </c>
@@ -1781,7 +1783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>83</v>
       </c>
@@ -1795,7 +1797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>85</v>
       </c>
@@ -1809,7 +1811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>133</v>
       </c>
@@ -1823,7 +1825,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>87</v>
       </c>
@@ -1837,7 +1839,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>89</v>
       </c>
@@ -1851,7 +1853,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>135</v>
       </c>
@@ -1865,7 +1867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>91</v>
       </c>
@@ -1879,7 +1881,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>93</v>
       </c>
@@ -1893,7 +1895,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>137</v>
       </c>
@@ -1907,7 +1909,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>139</v>
       </c>
@@ -1921,7 +1923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>95</v>
       </c>
@@ -1935,7 +1937,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>97</v>
       </c>
@@ -1949,7 +1951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>141</v>
       </c>
@@ -1963,7 +1965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>143</v>
       </c>
@@ -1977,7 +1979,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>145</v>
       </c>
@@ -1991,7 +1993,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>99</v>
       </c>
@@ -2005,7 +2007,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>147</v>
       </c>
@@ -2019,7 +2021,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>164</v>
       </c>
@@ -2033,7 +2035,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>101</v>
       </c>
@@ -2047,7 +2049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>149</v>
       </c>
@@ -2061,7 +2063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>151</v>
       </c>
@@ -2075,7 +2077,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>174</v>
       </c>

</xml_diff>

<commit_message>
created a shortlist of countries for future work
</commit_message>
<xml_diff>
--- a/misc/population.xlsx
+++ b/misc/population.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashok\Desktop\spatialEpisim2022\spatialEpisim\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cupcake\Documents\MRU\Year 4\Winter\Senior Project\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF4AABE-E8BA-4475-8169-02F59F197040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A3F817-A15E-4F90-BE91-4F9843233CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
   <si>
     <t>Country</t>
   </si>
@@ -559,6 +559,9 @@
   </si>
   <si>
     <t>ZWE</t>
+  </si>
+  <si>
+    <t>shortList</t>
   </si>
 </sst>
 </file>
@@ -858,22 +861,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C5C62-C8EE-4F49-9292-237310EC5B94}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="1"/>
+    <col min="3" max="3" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -886,8 +890,11 @@
       <c r="D1" s="3" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>158</v>
       </c>
@@ -900,8 +907,11 @@
       <c r="D2" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>103</v>
       </c>
@@ -914,8 +924,11 @@
       <c r="D3" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -928,8 +941,11 @@
       <c r="D4" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>160</v>
       </c>
@@ -942,8 +958,11 @@
       <c r="D5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -956,8 +975,11 @@
       <c r="D6" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -970,8 +992,11 @@
       <c r="D7" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -984,8 +1009,11 @@
       <c r="D8" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -998,8 +1026,11 @@
       <c r="D9" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -1012,8 +1043,11 @@
       <c r="D10" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>105</v>
       </c>
@@ -1026,8 +1060,11 @@
       <c r="D11" s="4">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E11" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -1040,8 +1077,11 @@
       <c r="D12" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -1054,8 +1094,11 @@
       <c r="D13" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -1068,8 +1111,11 @@
       <c r="D14" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E14" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>1</v>
       </c>
@@ -1082,8 +1128,11 @@
       <c r="D15" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1096,8 +1145,11 @@
       <c r="D16" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
@@ -1110,8 +1162,11 @@
       <c r="D17" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>162</v>
       </c>
@@ -1124,8 +1179,11 @@
       <c r="D18" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E18" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
@@ -1138,8 +1196,11 @@
       <c r="D19" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>107</v>
       </c>
@@ -1152,8 +1213,11 @@
       <c r="D20" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1166,8 +1230,11 @@
       <c r="D21" s="4">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E21" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
@@ -1180,8 +1247,11 @@
       <c r="D22" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E22" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>109</v>
       </c>
@@ -1194,8 +1264,11 @@
       <c r="D23" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
@@ -1208,8 +1281,11 @@
       <c r="D24" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E24" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>166</v>
       </c>
@@ -1222,8 +1298,11 @@
       <c r="D25" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E25" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
@@ -1236,8 +1315,11 @@
       <c r="D26" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E26" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>111</v>
       </c>
@@ -1250,8 +1332,11 @@
       <c r="D27" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E27" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>41</v>
       </c>
@@ -1264,8 +1349,11 @@
       <c r="D28" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E28" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>168</v>
       </c>
@@ -1278,8 +1366,11 @@
       <c r="D29" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E29" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>43</v>
       </c>
@@ -1292,8 +1383,11 @@
       <c r="D30" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E30" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>45</v>
       </c>
@@ -1306,8 +1400,11 @@
       <c r="D31" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E31" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>47</v>
       </c>
@@ -1320,8 +1417,11 @@
       <c r="D32" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E32" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>49</v>
       </c>
@@ -1334,8 +1434,11 @@
       <c r="D33" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E33" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>170</v>
       </c>
@@ -1348,8 +1451,11 @@
       <c r="D34" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E34" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>51</v>
       </c>
@@ -1362,8 +1468,11 @@
       <c r="D35" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E35" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>113</v>
       </c>
@@ -1376,8 +1485,11 @@
       <c r="D36" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E36" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>53</v>
       </c>
@@ -1390,8 +1502,11 @@
       <c r="D37" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E37" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -1404,8 +1519,11 @@
       <c r="D38" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E38" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>154</v>
       </c>
@@ -1418,8 +1536,11 @@
       <c r="D39" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E39" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>116</v>
       </c>
@@ -1432,8 +1553,11 @@
       <c r="D40" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E40" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>55</v>
       </c>
@@ -1446,8 +1570,11 @@
       <c r="D41" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E41" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>117</v>
       </c>
@@ -1460,8 +1587,11 @@
       <c r="D42" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E42" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>57</v>
       </c>
@@ -1474,8 +1604,11 @@
       <c r="D43" s="4">
         <v>25</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E43" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>119</v>
       </c>
@@ -1488,8 +1621,11 @@
       <c r="D44" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E44" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>59</v>
       </c>
@@ -1502,8 +1638,11 @@
       <c r="D45" s="4">
         <v>55</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E45" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>121</v>
       </c>
@@ -1516,8 +1655,11 @@
       <c r="D46" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E46" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>123</v>
       </c>
@@ -1530,8 +1672,11 @@
       <c r="D47" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E47" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>125</v>
       </c>
@@ -1544,8 +1689,11 @@
       <c r="D48" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E48" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>61</v>
       </c>
@@ -1558,8 +1706,11 @@
       <c r="D49" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E49" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>127</v>
       </c>
@@ -1572,8 +1723,11 @@
       <c r="D50" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E50" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>5</v>
       </c>
@@ -1586,8 +1740,11 @@
       <c r="D51" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E51" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>155</v>
       </c>
@@ -1600,8 +1757,11 @@
       <c r="D52" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E52" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>63</v>
       </c>
@@ -1614,8 +1774,11 @@
       <c r="D53" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E53" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>65</v>
       </c>
@@ -1628,8 +1791,11 @@
       <c r="D54" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E54" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>172</v>
       </c>
@@ -1642,8 +1808,11 @@
       <c r="D55" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E55" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>67</v>
       </c>
@@ -1656,8 +1825,11 @@
       <c r="D56" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E56" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>69</v>
       </c>
@@ -1670,8 +1842,11 @@
       <c r="D57" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E57" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>71</v>
       </c>
@@ -1684,8 +1859,11 @@
       <c r="D58" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E58" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>73</v>
       </c>
@@ -1698,8 +1876,11 @@
       <c r="D59" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E59" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>75</v>
       </c>
@@ -1712,8 +1893,11 @@
       <c r="D60" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E60" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>77</v>
       </c>
@@ -1726,8 +1910,11 @@
       <c r="D61" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E61" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>129</v>
       </c>
@@ -1740,8 +1927,11 @@
       <c r="D62" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E62" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>79</v>
       </c>
@@ -1754,8 +1944,11 @@
       <c r="D63" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E63" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>131</v>
       </c>
@@ -1768,8 +1961,11 @@
       <c r="D64" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E64" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>81</v>
       </c>
@@ -1782,8 +1978,11 @@
       <c r="D65" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E65" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>83</v>
       </c>
@@ -1796,8 +1995,11 @@
       <c r="D66" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E66" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>85</v>
       </c>
@@ -1810,8 +2012,11 @@
       <c r="D67" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E67" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>133</v>
       </c>
@@ -1824,8 +2029,11 @@
       <c r="D68" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E68" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>87</v>
       </c>
@@ -1838,8 +2046,11 @@
       <c r="D69" s="4">
         <v>55</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E69" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>89</v>
       </c>
@@ -1852,8 +2063,11 @@
       <c r="D70" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E70" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>135</v>
       </c>
@@ -1866,8 +2080,11 @@
       <c r="D71" s="4">
         <v>25</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E71" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>91</v>
       </c>
@@ -1880,8 +2097,11 @@
       <c r="D72" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E72" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>93</v>
       </c>
@@ -1894,8 +2114,11 @@
       <c r="D73" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E73" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>137</v>
       </c>
@@ -1908,8 +2131,11 @@
       <c r="D74" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E74" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>139</v>
       </c>
@@ -1922,8 +2148,11 @@
       <c r="D75" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E75" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>95</v>
       </c>
@@ -1936,8 +2165,11 @@
       <c r="D76" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E76" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>97</v>
       </c>
@@ -1950,8 +2182,11 @@
       <c r="D77" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E77" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>141</v>
       </c>
@@ -1964,8 +2199,11 @@
       <c r="D78" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E78" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>143</v>
       </c>
@@ -1978,8 +2216,11 @@
       <c r="D79" s="4">
         <v>25</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E79" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>145</v>
       </c>
@@ -1992,8 +2233,11 @@
       <c r="D80" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E80" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>99</v>
       </c>
@@ -2006,8 +2250,11 @@
       <c r="D81" s="4">
         <v>25</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E81" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>147</v>
       </c>
@@ -2020,8 +2267,11 @@
       <c r="D82" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E82" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>164</v>
       </c>
@@ -2034,8 +2284,11 @@
       <c r="D83" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E83" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>101</v>
       </c>
@@ -2048,8 +2301,11 @@
       <c r="D84" s="4">
         <v>25</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E84" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>149</v>
       </c>
@@ -2062,8 +2318,11 @@
       <c r="D85" s="4">
         <v>25</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E85" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>151</v>
       </c>
@@ -2076,8 +2335,11 @@
       <c r="D86" s="4">
         <v>25</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E86" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>174</v>
       </c>
@@ -2089,6 +2351,9 @@
       </c>
       <c r="D87" s="4">
         <v>15</v>
+      </c>
+      <c r="E87" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added South Africa and South Korea to shortlist
</commit_message>
<xml_diff>
--- a/misc/population.xlsx
+++ b/misc/population.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cupcake\Documents\MRU\Year 4\Winter\Senior Project\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A3F817-A15E-4F90-BE91-4F9843233CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19307E6-B0FD-42B1-A98F-8B83BEFA6461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C5C62-C8EE-4F49-9292-237310EC5B94}">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2047,7 +2047,7 @@
         <v>55</v>
       </c>
       <c r="E69" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -2064,7 +2064,7 @@
         <v>15</v>
       </c>
       <c r="E70" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>